<commit_message>
Atualiza modelo logico, fisico, inserção de dados
</commit_message>
<xml_diff>
--- a/arquivos/planilhas/tabela_normalizada.xlsx
+++ b/arquivos/planilhas/tabela_normalizada.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="ALOCA" sheetId="14" r:id="rId1"/>
-    <sheet name="MOTORISTA" sheetId="13" r:id="rId2"/>
-    <sheet name="CAMINHAO" sheetId="3" r:id="rId3"/>
+    <sheet name="CAMINHAO" sheetId="3" r:id="rId2"/>
+    <sheet name="MOTORISTA" sheetId="13" r:id="rId3"/>
     <sheet name="MARCA" sheetId="1" r:id="rId4"/>
     <sheet name="MODELO" sheetId="2" r:id="rId5"/>
     <sheet name="BAIRRO" sheetId="4" r:id="rId6"/>
@@ -95,39 +95,6 @@
     <t>CAPACIDADE</t>
   </si>
   <si>
-    <t>MTR-3338</t>
-  </si>
-  <si>
-    <t>MTV-4311</t>
-  </si>
-  <si>
-    <t>MQZ-8687</t>
-  </si>
-  <si>
-    <t>MTB-1361</t>
-  </si>
-  <si>
-    <t>MSG-4883</t>
-  </si>
-  <si>
-    <t>MSZ-7251</t>
-  </si>
-  <si>
-    <t>MRB-6206</t>
-  </si>
-  <si>
-    <t>MRY-5351</t>
-  </si>
-  <si>
-    <t>MRF-7474</t>
-  </si>
-  <si>
-    <t>MSI-6750</t>
-  </si>
-  <si>
-    <t>MRP-5441</t>
-  </si>
-  <si>
     <t>COD_BAIRRO</t>
   </si>
   <si>
@@ -329,6 +296,39 @@
   </si>
   <si>
     <t>HORA_FIM</t>
+  </si>
+  <si>
+    <t>MTR3338</t>
+  </si>
+  <si>
+    <t>MTV4311</t>
+  </si>
+  <si>
+    <t>MQZ8687</t>
+  </si>
+  <si>
+    <t>MTB1361</t>
+  </si>
+  <si>
+    <t>MSG4883</t>
+  </si>
+  <si>
+    <t>MSZ7251</t>
+  </si>
+  <si>
+    <t>MRB6206</t>
+  </si>
+  <si>
+    <t>MRY5351</t>
+  </si>
+  <si>
+    <t>MRF7474</t>
+  </si>
+  <si>
+    <t>MSI6750</t>
+  </si>
+  <si>
+    <t>MRP5441</t>
   </si>
 </sst>
 </file>
@@ -868,9 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -885,19 +883,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1028,19 +1026,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2016,10 +2014,10 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2270,10 +2268,10 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2296,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="3"/>
@@ -2319,7 +2317,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3"/>
@@ -2342,7 +2340,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
@@ -2367,6 +2365,292 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="20" width="8.5703125" customWidth="1"/>
+    <col min="21" max="1018" width="14.140625" customWidth="1"/>
+    <col min="1019" max="1025" width="11.5703125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-20.1961361</v>
+      </c>
+      <c r="D2" s="9">
+        <v>-40.2555063</v>
+      </c>
+      <c r="E2" s="37">
+        <v>11000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-20.198240299999998</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-40.253086099999997</v>
+      </c>
+      <c r="E3" s="37">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="9">
+        <v>-20.198687499999998</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-40.258083499999998</v>
+      </c>
+      <c r="E4" s="37">
+        <v>12100</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="9">
+        <v>-20.1959193</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-40.258790400000002</v>
+      </c>
+      <c r="E5" s="37">
+        <v>11000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-20.192520500000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-40.2568421</v>
+      </c>
+      <c r="E6" s="37">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-20.193270600000002</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-40.252901299999998</v>
+      </c>
+      <c r="E7" s="37">
+        <v>12000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-20.195081200000001</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-40.251535199999999</v>
+      </c>
+      <c r="E8" s="37">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-20.196940900000001</v>
+      </c>
+      <c r="D9" s="9">
+        <v>-40.2516228</v>
+      </c>
+      <c r="E9" s="37">
+        <v>12000</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="9">
+        <v>-20.196940900000001</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-40.251292800000002</v>
+      </c>
+      <c r="E10" s="7">
+        <v>12100</v>
+      </c>
+      <c r="F10" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-20.193110600000001</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-40.200552799999997</v>
+      </c>
+      <c r="E11" s="7">
+        <v>14000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-20.195211199999999</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-40.255896300000003</v>
+      </c>
+      <c r="E12" s="7">
+        <v>14000</v>
+      </c>
+      <c r="F12" s="7">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -2386,13 +2670,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2404,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C2" s="5">
         <v>79422697522</v>
@@ -2418,7 +2702,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5">
         <v>32137438011</v>
@@ -2432,7 +2716,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5">
         <v>85592912563</v>
@@ -2446,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C5" s="5">
         <v>54883575163</v>
@@ -2460,7 +2744,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5">
         <v>57614486347</v>
@@ -2474,7 +2758,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C7" s="5">
         <v>75366268453</v>
@@ -2488,7 +2772,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>61646505787</v>
@@ -2499,296 +2783,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>98624129824</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="20" width="8.5703125" customWidth="1"/>
-    <col min="21" max="1018" width="14.140625" customWidth="1"/>
-    <col min="1019" max="1025" width="11.5703125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-20.1961361</v>
-      </c>
-      <c r="D2" s="9">
-        <v>-40.2555063</v>
-      </c>
-      <c r="E2" s="37">
-        <v>11000</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="9">
-        <v>-20.198240299999998</v>
-      </c>
-      <c r="D3" s="9">
-        <v>-40.253086099999997</v>
-      </c>
-      <c r="E3" s="37">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="4">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="9">
-        <v>-20.198687499999998</v>
-      </c>
-      <c r="D4" s="9">
-        <v>-40.258083499999998</v>
-      </c>
-      <c r="E4" s="37">
-        <v>12100</v>
-      </c>
-      <c r="F4" s="4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="9">
-        <v>-20.1959193</v>
-      </c>
-      <c r="D5" s="9">
-        <v>-40.258790400000002</v>
-      </c>
-      <c r="E5" s="37">
-        <v>11000</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="9">
-        <v>-20.192520500000001</v>
-      </c>
-      <c r="D6" s="9">
-        <v>-40.2568421</v>
-      </c>
-      <c r="E6" s="37">
-        <v>10000</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="9">
-        <v>-20.193270600000002</v>
-      </c>
-      <c r="D7" s="9">
-        <v>-40.252901299999998</v>
-      </c>
-      <c r="E7" s="37">
-        <v>12000</v>
-      </c>
-      <c r="F7" s="4">
-        <v>5</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="9">
-        <v>-20.195081200000001</v>
-      </c>
-      <c r="D8" s="9">
-        <v>-40.251535199999999</v>
-      </c>
-      <c r="E8" s="37">
-        <v>10000</v>
-      </c>
-      <c r="F8" s="7">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="9">
-        <v>-20.196940900000001</v>
-      </c>
-      <c r="D9" s="9">
-        <v>-40.2516228</v>
-      </c>
-      <c r="E9" s="37">
-        <v>12000</v>
-      </c>
-      <c r="F9" s="7">
-        <v>6</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="9">
-        <v>-20.196940900000001</v>
-      </c>
-      <c r="D10" s="9">
-        <v>-40.251292800000002</v>
-      </c>
-      <c r="E10" s="7">
-        <v>12100</v>
-      </c>
-      <c r="F10" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="9">
-        <v>-20.193110600000001</v>
-      </c>
-      <c r="D11" s="9">
-        <v>-40.200552799999997</v>
-      </c>
-      <c r="E11" s="7">
-        <v>14000</v>
-      </c>
-      <c r="F11" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="9">
-        <v>-20.195211199999999</v>
-      </c>
-      <c r="D12" s="9">
-        <v>-40.255896300000003</v>
-      </c>
-      <c r="E12" s="7">
-        <v>14000</v>
-      </c>
-      <c r="F12" s="7">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3069,10 +3067,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3080,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3088,7 +3086,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3096,7 +3094,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3104,7 +3102,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3112,7 +3110,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3120,7 +3118,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3166,16 +3164,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -3189,13 +3187,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E2" s="14">
         <v>-20.050771130000001</v>
@@ -3209,13 +3207,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E3" s="14">
         <v>-20.086888510000001</v>
@@ -3229,13 +3227,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E4" s="14">
         <v>-20.200346010000001</v>
@@ -3249,13 +3247,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E5" s="14">
         <v>-20.26219712</v>
@@ -3269,13 +3267,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E6" s="14">
         <v>-20.390974409999998</v>
@@ -3289,13 +3287,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E7" s="14">
         <v>-20.205501210000001</v>
@@ -3309,13 +3307,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E8" s="14">
         <v>-20.174567450000001</v>
@@ -3329,13 +3327,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E9" s="14">
         <v>-20.295045510000001</v>
@@ -3349,13 +3347,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E10" s="14">
         <v>-19.295045510000001</v>
@@ -3369,13 +3367,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E11" s="14">
         <v>-18.293045509999999</v>
@@ -3415,10 +3413,10 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>18</v>
@@ -4133,22 +4131,22 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>